<commit_message>
WP1 Demo and tidy up
Also minor tweaks
</commit_message>
<xml_diff>
--- a/input-data/Infra Selection Rules.xlsx
+++ b/input-data/Infra Selection Rules.xlsx
@@ -296,7 +296,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -385,12 +385,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -408,16 +402,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -433,6 +421,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -723,7 +723,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="H21:M21"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -743,46 +743,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -832,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2">
         <v>150</v>
@@ -849,19 +849,19 @@
       <c r="G3" s="2">
         <v>999999</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>2.5</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <v>1.5</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <v>3.5</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="10">
         <v>3</v>
       </c>
       <c r="M3" t="s">
@@ -890,19 +890,19 @@
       <c r="G4" s="2">
         <v>999999</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>3</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="8">
         <v>2.5</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="8">
         <v>3.5</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="10">
         <v>3</v>
       </c>
       <c r="M4" t="s">
@@ -931,19 +931,19 @@
       <c r="G5" s="2">
         <v>999999</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>4</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <v>3.5</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="8">
         <v>3.5</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="10">
         <v>3</v>
       </c>
       <c r="M5" t="s">
@@ -955,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2">
         <v>150</v>
@@ -972,19 +972,19 @@
       <c r="G6" s="2">
         <v>999999</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>2.5</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <v>1.5</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="8">
         <v>2.5</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="10">
         <v>2</v>
       </c>
       <c r="M6" t="s">
@@ -1013,19 +1013,19 @@
       <c r="G7" s="2">
         <v>999999</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <v>3</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <v>2.5</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="8">
         <v>2.5</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="10">
         <v>2</v>
       </c>
       <c r="M7" t="s">
@@ -1054,19 +1054,19 @@
       <c r="G8" s="2">
         <v>999999</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <v>4</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="8">
         <v>3.5</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="8">
         <v>2.5</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="10">
         <v>2</v>
       </c>
       <c r="M8" t="s">
@@ -1078,7 +1078,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2">
         <v>150</v>
@@ -1095,19 +1095,19 @@
       <c r="G9" s="2">
         <v>999999</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <v>2.5</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="8">
         <v>1.5</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="8">
         <v>2</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="8">
         <v>1.5</v>
       </c>
       <c r="M9" t="s">
@@ -1136,19 +1136,19 @@
       <c r="G10" s="2">
         <v>999999</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="8">
         <v>3</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="8">
         <v>2.5</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="8">
         <v>2</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="8">
         <v>1.5</v>
       </c>
       <c r="M10" t="s">
@@ -1177,19 +1177,19 @@
       <c r="G11" s="2">
         <v>999999</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="8">
         <v>4</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="8">
         <v>3.5</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="8">
         <v>2</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="8">
         <v>1.5</v>
       </c>
       <c r="M11" t="s">
@@ -1201,7 +1201,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2">
         <v>150</v>
@@ -1218,19 +1218,19 @@
       <c r="G12" s="2">
         <v>999999</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="8">
         <v>2.5</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="8">
         <v>1.5</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="8">
         <v>1</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="8">
         <v>0.5</v>
       </c>
       <c r="M12" t="s">
@@ -1259,19 +1259,19 @@
       <c r="G13" s="2">
         <v>999999</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="8">
         <v>3</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="8">
         <v>2.5</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="8">
         <v>1</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="8">
         <v>0.5</v>
       </c>
       <c r="M13" t="s">
@@ -1300,19 +1300,19 @@
       <c r="G14" s="2">
         <v>999999</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <v>4</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <v>3.5</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="8">
         <v>1</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="8">
         <v>0.5</v>
       </c>
       <c r="M14" t="s">
@@ -1324,7 +1324,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2">
         <v>150</v>
@@ -1341,19 +1341,19 @@
       <c r="G15" s="2">
         <v>5000</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="8">
         <v>2</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="8">
         <v>1.5</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="8">
         <v>0.5</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="8">
         <v>0</v>
       </c>
       <c r="M15" t="s">
@@ -1382,19 +1382,19 @@
       <c r="G16" s="2">
         <v>5000</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <v>2</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="8">
         <v>1.5</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="8">
         <v>0.5</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="8">
         <v>0</v>
       </c>
       <c r="M16" t="s">
@@ -1423,19 +1423,19 @@
       <c r="G17" s="2">
         <v>5000</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>2.5</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>1.5</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="8">
         <v>0.5</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="8">
         <v>0</v>
       </c>
       <c r="M17" t="s">
@@ -1450,7 +1450,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2">
         <v>150</v>
@@ -1467,19 +1467,19 @@
       <c r="G18" s="2">
         <v>999999</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>2.5</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="8">
         <v>1.5</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="8">
         <v>0.5</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="8">
         <v>0</v>
       </c>
       <c r="M18" t="s">
@@ -1508,19 +1508,19 @@
       <c r="G19" s="2">
         <v>999999</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <v>3</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <v>2.5</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="8">
         <v>0.5</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="8">
         <v>0</v>
       </c>
       <c r="M19" t="s">
@@ -1549,19 +1549,19 @@
       <c r="G20" s="2">
         <v>999999</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="8">
         <v>4</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="8">
         <v>3.5</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="8">
         <v>0.5</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="8">
         <v>0</v>
       </c>
       <c r="M20" t="s">
@@ -1573,7 +1573,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2">
         <v>999999</v>
@@ -1590,19 +1590,19 @@
       <c r="G21" s="2">
         <v>2500</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="10">
-        <v>0</v>
-      </c>
-      <c r="J21" s="10">
-        <v>0</v>
-      </c>
-      <c r="K21" s="10">
-        <v>0</v>
-      </c>
-      <c r="L21" s="10">
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
         <v>0</v>
       </c>
       <c r="M21" t="s">
@@ -1614,7 +1614,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2">
         <v>150</v>
@@ -1631,19 +1631,19 @@
       <c r="G22" s="2">
         <v>5000</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="8">
         <v>2</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="8">
         <v>1.5</v>
       </c>
-      <c r="K22" s="10">
-        <v>0</v>
-      </c>
-      <c r="L22" s="10">
+      <c r="K22" s="8">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8">
         <v>0</v>
       </c>
       <c r="M22" t="s">
@@ -1672,19 +1672,19 @@
       <c r="G23" s="2">
         <v>5000</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" s="10">
+      <c r="H23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="8">
         <v>2.5</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="8">
         <v>1.5</v>
       </c>
-      <c r="K23" s="10">
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
+      <c r="K23" s="8">
+        <v>0</v>
+      </c>
+      <c r="L23" s="8">
         <v>0</v>
       </c>
       <c r="M23" t="s">
@@ -1699,7 +1699,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2">
         <v>150</v>
@@ -1716,19 +1716,19 @@
       <c r="G24" s="2">
         <v>999999</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="8">
         <v>2.5</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="8">
         <v>1.5</v>
       </c>
-      <c r="K24" s="10">
-        <v>0</v>
-      </c>
-      <c r="L24" s="10">
+      <c r="K24" s="8">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
         <v>0</v>
       </c>
       <c r="M24" t="s">
@@ -1757,19 +1757,19 @@
       <c r="G25" s="2">
         <v>999999</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="8">
         <v>3</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="8">
         <v>2.5</v>
       </c>
-      <c r="K25" s="10">
-        <v>0</v>
-      </c>
-      <c r="L25" s="10">
+      <c r="K25" s="8">
+        <v>0</v>
+      </c>
+      <c r="L25" s="8">
         <v>0</v>
       </c>
       <c r="M25" t="s">
@@ -1798,19 +1798,19 @@
       <c r="G26" s="2">
         <v>999999</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="8">
         <v>4</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="8">
         <v>3.5</v>
       </c>
-      <c r="K26" s="10">
-        <v>0</v>
-      </c>
-      <c r="L26" s="10">
+      <c r="K26" s="8">
+        <v>0</v>
+      </c>
+      <c r="L26" s="8">
         <v>0</v>
       </c>
       <c r="M26" t="s">
@@ -1843,74 +1843,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="18">
         <v>30</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="18">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1935,108 +1935,108 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2046,63 +2046,63 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="19"/>
     </row>
     <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -2110,13 +2110,13 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2124,10 +2124,10 @@
       <c r="A35" s="2">
         <v>30</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="8">
         <v>0.5</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2135,10 +2135,10 @@
       <c r="A36" s="2">
         <v>40</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="8">
         <v>1</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -2146,10 +2146,10 @@
       <c r="A37" s="2">
         <v>50</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2157,10 +2157,10 @@
       <c r="A38" s="2">
         <v>60</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2168,10 +2168,10 @@
       <c r="A39" s="2">
         <v>70</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>